<commit_message>
Update documentation files (manual add)
</commit_message>
<xml_diff>
--- a/Documentation/Quality_Control.xlsx
+++ b/Documentation/Quality_Control.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Electronica Care\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\pet\petAdoption_SWPM\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9392F7C-D0CE-4CE9-A32F-464A5A153D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="1644" windowWidth="8040" windowHeight="8556" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="1644" windowWidth="8040" windowHeight="8556"/>
   </bookViews>
   <sheets>
     <sheet name="Quality Control Template" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t xml:space="preserve">    Quality Control</t>
   </si>
@@ -142,12 +141,39 @@
   </si>
   <si>
     <t>Responivenes on Small Screens</t>
+  </si>
+  <si>
+    <t>Notification Alerts</t>
+  </si>
+  <si>
+    <t>Notifications don't disappear automatically after being read</t>
+  </si>
+  <si>
+    <t>Pet Profile Editing</t>
+  </si>
+  <si>
+    <t>Editing pet profile image causes layout distortion</t>
+  </si>
+  <si>
+    <t>Admin Panel Access</t>
+  </si>
+  <si>
+    <t>Some admin users can't access the dashboard</t>
+  </si>
+  <si>
+    <t>Related to role settings</t>
+  </si>
+  <si>
+    <t>Chat Timestamp Format</t>
+  </si>
+  <si>
+    <t>Timestamps in chat are inconsistent across time zones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -244,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -262,11 +288,615 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="74">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAEABAB"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAEABAB"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAEABAB"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFAEABAB"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9887"/>
+          <bgColor rgb="FFFF9887"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -531,17 +1161,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="2" max="2" width="50.3984375" customWidth="1"/>
     <col min="3" max="3" width="14.19921875" customWidth="1"/>
     <col min="4" max="4" width="13.8984375" customWidth="1"/>
     <col min="5" max="5" width="19.19921875" customWidth="1"/>
@@ -916,52 +1546,117 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="A13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="11">
+        <v>45791</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="6">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="11">
+        <v>45790</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="A15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="6">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="11">
+        <v>45791</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="A16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="11">
+        <v>45791</v>
+      </c>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
@@ -2563,7 +3258,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="C4:C24">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="formula" val="45311"/>
         <cfvo type="max"/>
@@ -2572,38 +3267,148 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I49">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Critical">
+  <conditionalFormatting sqref="F4:I12 F17:I49">
+    <cfRule type="containsText" dxfId="73" priority="24" operator="containsText" text="Critical">
       <formula>NOT(ISERROR(SEARCH(("Critical"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I49">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="High">
+  <conditionalFormatting sqref="F4:I12 F17:I49">
+    <cfRule type="containsText" dxfId="72" priority="25" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH(("High"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I49">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Medium">
+  <conditionalFormatting sqref="F4:I12 F17:I49">
+    <cfRule type="containsText" dxfId="71" priority="26" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH(("Medium"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:I49">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Low">
+  <conditionalFormatting sqref="F4:I12 F17:I49">
+    <cfRule type="containsText" dxfId="70" priority="27" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH(("Low"),(F4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G49">
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Closed">
+  <conditionalFormatting sqref="G4:G12 G17:G49">
+    <cfRule type="containsText" dxfId="69" priority="28" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH(("Closed"),(G4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G49">
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Open">
+  <conditionalFormatting sqref="G4:G12 G17:G49">
+    <cfRule type="containsText" dxfId="68" priority="29" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH(("Open"),(G4))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="containsText" dxfId="63" priority="19" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH(("Critical"),(F13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="containsText" dxfId="61" priority="20" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH(("High"),(F13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="containsText" dxfId="59" priority="21" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH(("Medium"),(F13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="containsText" dxfId="57" priority="22" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH(("Low"),(F13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="containsText" dxfId="55" priority="15" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH(("Critical"),(F14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="containsText" dxfId="53" priority="16" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH(("High"),(F14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="containsText" dxfId="51" priority="17" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH(("Medium"),(F14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="containsText" dxfId="49" priority="18" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH(("Low"),(F14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="containsText" dxfId="43" priority="11" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH(("Critical"),(F15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="containsText" dxfId="41" priority="12" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH(("High"),(F15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="containsText" dxfId="39" priority="13" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH(("Medium"),(F15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH(("Low"),(F15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH(("Critical"),(F16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH(("High"),(F16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH(("Medium"),(F16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH(("Low"),(F16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G16">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH(("Critical"),(G13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G16">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH(("High"),(G13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G16">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH(("Medium"),(G13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G16">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH(("Low"),(G13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G16">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH(("Closed"),(G13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G16">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH(("Open"),(G13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C24">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>